<commit_message>
docs: update i18n docs
</commit_message>
<xml_diff>
--- a/lang.xlsx
+++ b/lang.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:ns4="http://schemas.microsoft.com/office/excel/2006/main" xmlns:ns5="http://schemas.microsoft.com/office/excel/2008/2/main" count="1391" uniqueCount="1391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:ns4="http://schemas.microsoft.com/office/excel/2006/main" xmlns:ns5="http://schemas.microsoft.com/office/excel/2008/2/main" count="1427" uniqueCount="1427">
   <si>
     <t>key</t>
   </si>
@@ -3503,61 +3503,169 @@
     <t>trans0469</t>
   </si>
   <si>
+    <t>IPv6 %s 配置</t>
+  </si>
+  <si>
+    <t>IPv6 %s Configuration</t>
+  </si>
+  <si>
     <t>trans0470</t>
   </si>
   <si>
+    <t>如果一个IPv6地址的首选寿命到期了，一般都禁止使用这个地址来启动新的连接</t>
+  </si>
+  <si>
+    <t>If the primary time of IPv6 address expire, it will be prohibited to start the new connection</t>
+  </si>
+  <si>
     <t>trans0471</t>
   </si>
   <si>
+    <t>SLAAC</t>
+  </si>
+  <si>
     <t>trans0472</t>
   </si>
   <si>
+    <t>DHCP</t>
+  </si>
+  <si>
     <t>trans0473</t>
   </si>
   <si>
+    <t>DNS</t>
+  </si>
+  <si>
     <t>trans0474</t>
   </si>
   <si>
+    <t>%s 状态</t>
+  </si>
+  <si>
+    <t>%s Status</t>
+  </si>
+  <si>
     <t>trans0475</t>
   </si>
   <si>
+    <t>RA 模式</t>
+  </si>
+  <si>
+    <t>RA Mode</t>
+  </si>
+  <si>
     <t>trans0476</t>
   </si>
   <si>
+    <t>前缀</t>
+  </si>
+  <si>
+    <t>Prefix</t>
+  </si>
+  <si>
     <t>trans0477</t>
   </si>
   <si>
+    <t>前缀长度</t>
+  </si>
+  <si>
+    <t>Prefix Length</t>
+  </si>
+  <si>
     <t>trans0478</t>
   </si>
   <si>
+    <t>首选寿命</t>
+  </si>
+  <si>
+    <t>Preferred Lifetime</t>
+  </si>
+  <si>
     <t>trans0479</t>
   </si>
   <si>
+    <t xml:space="preserve">有效寿命	</t>
+  </si>
+  <si>
+    <t>Valid Lifetime</t>
+  </si>
+  <si>
     <t>trans0480</t>
   </si>
   <si>
+    <t>RA 消息最小间隔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA minimum interval   </t>
+  </si>
+  <si>
     <t>trans0481</t>
   </si>
   <si>
+    <t>RA 消息最大间隔</t>
+  </si>
+  <si>
+    <t>RA maximal interval</t>
+  </si>
+  <si>
     <t>trans0482</t>
   </si>
   <si>
+    <t>MTU</t>
+  </si>
+  <si>
     <t>trans0483</t>
   </si>
   <si>
+    <t xml:space="preserve">Managed 标志  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Managed Flag  </t>
+  </si>
+  <si>
     <t>trans0484</t>
   </si>
   <si>
+    <t xml:space="preserve">Other 标志 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other Flag </t>
+  </si>
+  <si>
     <t>trans0485</t>
   </si>
   <si>
+    <t>前缀来源</t>
+  </si>
+  <si>
+    <t>Prefix Source</t>
+  </si>
+  <si>
     <t>trans0486</t>
   </si>
   <si>
+    <t>手动配置</t>
+  </si>
+  <si>
+    <t>Manually</t>
+  </si>
+  <si>
     <t>trans0487</t>
   </si>
   <si>
+    <t>自动配置</t>
+  </si>
+  <si>
+    <t>Automatically</t>
+  </si>
+  <si>
     <t>trans0488</t>
+  </si>
+  <si>
+    <t>秒</t>
+  </si>
+  <si>
+    <t>second(s)</t>
   </si>
   <si>
     <t>trans0489</t>
@@ -5338,7 +5446,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>1234</v>
+        <v>1270</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -5376,10 +5484,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>1235</v>
+        <v>1271</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1236</v>
+        <v>1272</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>8</v>
@@ -5395,7 +5503,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>1237</v>
+        <v>1273</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
@@ -5414,13 +5522,13 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>1238</v>
+        <v>1274</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1239</v>
+        <v>1275</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>1240</v>
+        <v>1276</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -5531,10 +5639,10 @@
         <v>26</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1241</v>
+        <v>1277</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>1242</v>
+        <v>1278</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -5718,10 +5826,10 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>1243</v>
+        <v>1279</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1244</v>
+        <v>1280</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>54</v>
@@ -5737,10 +5845,10 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>1245</v>
+        <v>1281</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>1246</v>
+        <v>1282</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="2"/>
@@ -5754,10 +5862,10 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>1247</v>
+        <v>1283</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>1248</v>
+        <v>1284</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="2"/>
@@ -5771,10 +5879,10 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>1249</v>
+        <v>1285</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>1250</v>
+        <v>1286</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="2"/>
@@ -5788,10 +5896,10 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>1251</v>
+        <v>1287</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>1252</v>
+        <v>1288</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="2"/>
@@ -5805,10 +5913,10 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>1253</v>
+        <v>1289</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>1254</v>
+        <v>1290</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="2"/>
@@ -5822,7 +5930,7 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>1255</v>
+        <v>1291</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>55</v>
@@ -5839,10 +5947,10 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>1256</v>
+        <v>1292</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>1257</v>
+        <v>1293</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="2"/>
@@ -5856,10 +5964,10 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>1258</v>
+        <v>1294</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>1259</v>
+        <v>1295</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="2"/>
@@ -5873,10 +5981,10 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>1260</v>
+        <v>1296</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>1261</v>
+        <v>1297</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="2"/>
@@ -5890,10 +5998,10 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>1262</v>
+        <v>1298</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>1263</v>
+        <v>1299</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="2"/>
@@ -5907,10 +6015,10 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>1264</v>
+        <v>1300</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>1265</v>
+        <v>1301</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="2"/>
@@ -5924,10 +6032,10 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>1266</v>
+        <v>1302</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>1267</v>
+        <v>1303</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="2"/>
@@ -5941,10 +6049,10 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>1268</v>
+        <v>1304</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>1269</v>
+        <v>1305</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="2"/>
@@ -5958,10 +6066,10 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>1270</v>
+        <v>1306</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>1271</v>
+        <v>1307</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="2"/>
@@ -5975,10 +6083,10 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>1272</v>
+        <v>1308</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>1273</v>
+        <v>1309</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="2"/>
@@ -5992,10 +6100,10 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>1274</v>
+        <v>1310</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>1261</v>
+        <v>1297</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="2"/>
@@ -6009,10 +6117,10 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>1275</v>
+        <v>1311</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>1276</v>
+        <v>1312</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="2"/>
@@ -6026,10 +6134,10 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>1277</v>
+        <v>1313</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>1278</v>
+        <v>1314</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="2"/>
@@ -6043,10 +6151,10 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>1279</v>
+        <v>1315</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>1280</v>
+        <v>1316</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="2"/>
@@ -6060,10 +6168,10 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>1281</v>
+        <v>1317</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>1282</v>
+        <v>1318</v>
       </c>
       <c r="C42" s="7"/>
       <c r="D42" s="2"/>
@@ -6077,10 +6185,10 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>1283</v>
+        <v>1319</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>1284</v>
+        <v>1320</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="2"/>
@@ -6094,10 +6202,10 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>1285</v>
+        <v>1321</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>1286</v>
+        <v>1322</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="2"/>
@@ -6111,10 +6219,10 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>1287</v>
+        <v>1323</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>1288</v>
+        <v>1324</v>
       </c>
       <c r="C45" s="7"/>
       <c r="D45" s="2"/>
@@ -6128,10 +6236,10 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>1289</v>
+        <v>1325</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>1290</v>
+        <v>1326</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="2"/>
@@ -6145,10 +6253,10 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>1291</v>
+        <v>1327</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>1292</v>
+        <v>1328</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="2"/>
@@ -6162,10 +6270,10 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>1293</v>
+        <v>1329</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>1294</v>
+        <v>1330</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="2"/>
@@ -6179,10 +6287,10 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>1295</v>
+        <v>1331</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>1246</v>
+        <v>1282</v>
       </c>
       <c r="C49" s="7"/>
       <c r="D49" s="2"/>
@@ -6196,13 +6304,13 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>1296</v>
+        <v>1332</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>1297</v>
+        <v>1333</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>1297</v>
+        <v>1333</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -6215,13 +6323,13 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>1298</v>
+        <v>1334</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>1299</v>
+        <v>1335</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>1299</v>
+        <v>1335</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -6234,7 +6342,7 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>1300</v>
+        <v>1336</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>60</v>
@@ -6251,7 +6359,7 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>1301</v>
+        <v>1337</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>61</v>
@@ -6268,7 +6376,7 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>1302</v>
+        <v>1338</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>62</v>
@@ -6288,7 +6396,7 @@
         <v>64</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>1263</v>
+        <v>1299</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>58</v>
@@ -6383,10 +6491,10 @@
         <v>78</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>1303</v>
+        <v>1339</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>1303</v>
+        <v>1339</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -8285,7 +8393,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>1304</v>
+        <v>1340</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -8323,10 +8431,10 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>1305</v>
+        <v>1341</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1306</v>
+        <v>1342</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>8</v>
@@ -8342,7 +8450,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>1307</v>
+        <v>1343</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
@@ -8361,13 +8469,13 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>1308</v>
+        <v>1344</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1309</v>
+        <v>1345</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>1310</v>
+        <v>1346</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -8478,10 +8586,10 @@
         <v>26</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1311</v>
+        <v>1347</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>1312</v>
+        <v>1348</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -8665,10 +8773,10 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>1313</v>
+        <v>1349</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1314</v>
+        <v>1350</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>54</v>
@@ -8684,10 +8792,10 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>1315</v>
+        <v>1351</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>1316</v>
+        <v>1352</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="2"/>
@@ -8701,10 +8809,10 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>1317</v>
+        <v>1353</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>1318</v>
+        <v>1354</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="2"/>
@@ -8718,10 +8826,10 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>1319</v>
+        <v>1355</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>1320</v>
+        <v>1356</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="2"/>
@@ -8735,10 +8843,10 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>1321</v>
+        <v>1357</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>1322</v>
+        <v>1358</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="2"/>
@@ -8752,10 +8860,10 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>1323</v>
+        <v>1359</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>1324</v>
+        <v>1360</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="2"/>
@@ -8769,10 +8877,10 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>1325</v>
+        <v>1361</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>1326</v>
+        <v>1362</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>55</v>
@@ -8788,10 +8896,10 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>1327</v>
+        <v>1363</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>1328</v>
+        <v>1364</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="2"/>
@@ -8805,10 +8913,10 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>1329</v>
+        <v>1365</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>1330</v>
+        <v>1366</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>56</v>
@@ -8824,10 +8932,10 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>1331</v>
+        <v>1367</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>1332</v>
+        <v>1368</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>57</v>
@@ -8843,10 +8951,10 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>1333</v>
+        <v>1369</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>1334</v>
+        <v>1370</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>58</v>
@@ -8862,10 +8970,10 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>1335</v>
+        <v>1371</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>1336</v>
+        <v>1372</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="2"/>
@@ -8879,10 +8987,10 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>1337</v>
+        <v>1373</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>1338</v>
+        <v>1374</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="2"/>
@@ -8896,10 +9004,10 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>1339</v>
+        <v>1375</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>1340</v>
+        <v>1376</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="2"/>
@@ -8913,10 +9021,10 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>1341</v>
+        <v>1377</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>1342</v>
+        <v>1378</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="2"/>
@@ -8930,10 +9038,10 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>1343</v>
+        <v>1379</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>1344</v>
+        <v>1380</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="2"/>
@@ -8947,10 +9055,10 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>1345</v>
+        <v>1381</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>1346</v>
+        <v>1382</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>59</v>
@@ -8966,10 +9074,10 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>1347</v>
+        <v>1383</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>1348</v>
+        <v>1384</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="2"/>
@@ -8983,10 +9091,10 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>1349</v>
+        <v>1385</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>1350</v>
+        <v>1386</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="2"/>
@@ -9000,10 +9108,10 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>1351</v>
+        <v>1387</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>1352</v>
+        <v>1388</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="2"/>
@@ -9017,10 +9125,10 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>1353</v>
+        <v>1389</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>1354</v>
+        <v>1390</v>
       </c>
       <c r="C42" s="7"/>
       <c r="D42" s="2"/>
@@ -9034,10 +9142,10 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>1355</v>
+        <v>1391</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>1356</v>
+        <v>1392</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="2"/>
@@ -9051,10 +9159,10 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>1357</v>
+        <v>1393</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>1358</v>
+        <v>1394</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="2"/>
@@ -9068,10 +9176,10 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>1359</v>
+        <v>1395</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>1360</v>
+        <v>1396</v>
       </c>
       <c r="C45" s="7"/>
       <c r="D45" s="2"/>
@@ -9085,10 +9193,10 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>1361</v>
+        <v>1397</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>1362</v>
+        <v>1398</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="2"/>
@@ -9102,10 +9210,10 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>1363</v>
+        <v>1399</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>1364</v>
+        <v>1400</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="2"/>
@@ -9119,10 +9227,10 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>1365</v>
+        <v>1401</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>1366</v>
+        <v>1402</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="2"/>
@@ -9136,10 +9244,10 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>1367</v>
+        <v>1403</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>1368</v>
+        <v>1404</v>
       </c>
       <c r="C49" s="7"/>
       <c r="D49" s="2"/>
@@ -9153,10 +9261,10 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>1369</v>
+        <v>1405</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>1370</v>
+        <v>1406</v>
       </c>
       <c r="C50" s="7"/>
       <c r="D50" s="2"/>
@@ -9170,10 +9278,10 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>1371</v>
+        <v>1407</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>1372</v>
+        <v>1408</v>
       </c>
       <c r="C51" s="7"/>
       <c r="D51" s="2"/>
@@ -9187,7 +9295,7 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>1373</v>
+        <v>1409</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>60</v>
@@ -9204,7 +9312,7 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>1374</v>
+        <v>1410</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>61</v>
@@ -9221,7 +9329,7 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>1375</v>
+        <v>1411</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>62</v>
@@ -9522,10 +9630,10 @@
         <v>105</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>1376</v>
+        <v>1412</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>1377</v>
+        <v>1413</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
@@ -9541,10 +9649,10 @@
         <v>106</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>1378</v>
+        <v>1414</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>1379</v>
+        <v>1415</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
@@ -9560,10 +9668,10 @@
         <v>107</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>1380</v>
+        <v>1416</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>1381</v>
+        <v>1417</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
@@ -9579,10 +9687,10 @@
         <v>108</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>1382</v>
+        <v>1418</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>1383</v>
+        <v>1419</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
@@ -9598,10 +9706,10 @@
         <v>109</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>1384</v>
+        <v>1420</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>1385</v>
+        <v>1421</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
@@ -9617,10 +9725,10 @@
         <v>110</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>1386</v>
+        <v>1422</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>1387</v>
+        <v>1423</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
@@ -9636,10 +9744,10 @@
         <v>111</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>1388</v>
+        <v>1424</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>1389</v>
+        <v>1425</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
@@ -10382,7 +10490,7 @@
         <v>206</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>1390</v>
+        <v>1426</v>
       </c>
       <c r="C118" s="8" t="s">
         <v>207</v>
@@ -16926,8 +17034,12 @@
       <c r="A469" s="1" t="s">
         <v>1158</v>
       </c>
-      <c r="B469" s="2"/>
-      <c r="C469" s="2"/>
+      <c r="B469" s="8" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C469" s="8" t="s">
+        <v>1160</v>
+      </c>
       <c r="D469" s="2"/>
       <c r="E469" s="2"/>
       <c r="F469" s="2"/>
@@ -16939,10 +17051,14 @@
     </row>
     <row r="470">
       <c r="A470" s="1" t="s">
-        <v>1159</v>
-      </c>
-      <c r="B470" s="2"/>
-      <c r="C470" s="2"/>
+        <v>1161</v>
+      </c>
+      <c r="B470" s="8" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C470" s="8" t="s">
+        <v>1163</v>
+      </c>
       <c r="D470" s="2"/>
       <c r="E470" s="2"/>
       <c r="F470" s="2"/>
@@ -16954,10 +17070,14 @@
     </row>
     <row r="471">
       <c r="A471" s="1" t="s">
-        <v>1160</v>
-      </c>
-      <c r="B471" s="2"/>
-      <c r="C471" s="2"/>
+        <v>1164</v>
+      </c>
+      <c r="B471" s="8" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C471" s="8" t="s">
+        <v>1165</v>
+      </c>
       <c r="D471" s="2"/>
       <c r="E471" s="2"/>
       <c r="F471" s="2"/>
@@ -16969,10 +17089,14 @@
     </row>
     <row r="472">
       <c r="A472" s="1" t="s">
-        <v>1161</v>
-      </c>
-      <c r="B472" s="2"/>
-      <c r="C472" s="2"/>
+        <v>1166</v>
+      </c>
+      <c r="B472" s="8" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C472" s="8" t="s">
+        <v>1167</v>
+      </c>
       <c r="D472" s="2"/>
       <c r="E472" s="2"/>
       <c r="F472" s="2"/>
@@ -16984,10 +17108,14 @@
     </row>
     <row r="473">
       <c r="A473" s="1" t="s">
-        <v>1162</v>
-      </c>
-      <c r="B473" s="2"/>
-      <c r="C473" s="2"/>
+        <v>1168</v>
+      </c>
+      <c r="B473" s="8" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C473" s="8" t="s">
+        <v>1169</v>
+      </c>
       <c r="D473" s="2"/>
       <c r="E473" s="2"/>
       <c r="F473" s="2"/>
@@ -16999,10 +17127,14 @@
     </row>
     <row r="474">
       <c r="A474" s="1" t="s">
-        <v>1163</v>
-      </c>
-      <c r="B474" s="2"/>
-      <c r="C474" s="2"/>
+        <v>1170</v>
+      </c>
+      <c r="B474" s="8" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C474" s="8" t="s">
+        <v>1172</v>
+      </c>
       <c r="D474" s="2"/>
       <c r="E474" s="2"/>
       <c r="F474" s="2"/>
@@ -17014,10 +17146,14 @@
     </row>
     <row r="475">
       <c r="A475" s="1" t="s">
-        <v>1164</v>
-      </c>
-      <c r="B475" s="2"/>
-      <c r="C475" s="2"/>
+        <v>1173</v>
+      </c>
+      <c r="B475" s="8" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C475" s="8" t="s">
+        <v>1175</v>
+      </c>
       <c r="D475" s="2"/>
       <c r="E475" s="2"/>
       <c r="F475" s="2"/>
@@ -17029,10 +17165,14 @@
     </row>
     <row r="476">
       <c r="A476" s="1" t="s">
-        <v>1165</v>
-      </c>
-      <c r="B476" s="2"/>
-      <c r="C476" s="2"/>
+        <v>1176</v>
+      </c>
+      <c r="B476" s="8" t="s">
+        <v>1177</v>
+      </c>
+      <c r="C476" s="8" t="s">
+        <v>1178</v>
+      </c>
       <c r="D476" s="2"/>
       <c r="E476" s="2"/>
       <c r="F476" s="2"/>
@@ -17044,10 +17184,14 @@
     </row>
     <row r="477">
       <c r="A477" s="1" t="s">
-        <v>1166</v>
-      </c>
-      <c r="B477" s="2"/>
-      <c r="C477" s="2"/>
+        <v>1179</v>
+      </c>
+      <c r="B477" s="8" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C477" s="8" t="s">
+        <v>1181</v>
+      </c>
       <c r="D477" s="2"/>
       <c r="E477" s="2"/>
       <c r="F477" s="2"/>
@@ -17059,10 +17203,14 @@
     </row>
     <row r="478">
       <c r="A478" s="1" t="s">
-        <v>1167</v>
-      </c>
-      <c r="B478" s="2"/>
-      <c r="C478" s="2"/>
+        <v>1182</v>
+      </c>
+      <c r="B478" s="8" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C478" s="8" t="s">
+        <v>1184</v>
+      </c>
       <c r="D478" s="2"/>
       <c r="E478" s="2"/>
       <c r="F478" s="2"/>
@@ -17074,10 +17222,14 @@
     </row>
     <row r="479">
       <c r="A479" s="1" t="s">
-        <v>1168</v>
-      </c>
-      <c r="B479" s="2"/>
-      <c r="C479" s="2"/>
+        <v>1185</v>
+      </c>
+      <c r="B479" s="8" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C479" s="8" t="s">
+        <v>1187</v>
+      </c>
       <c r="D479" s="2"/>
       <c r="E479" s="2"/>
       <c r="F479" s="2"/>
@@ -17089,10 +17241,14 @@
     </row>
     <row r="480">
       <c r="A480" s="1" t="s">
-        <v>1169</v>
-      </c>
-      <c r="B480" s="2"/>
-      <c r="C480" s="2"/>
+        <v>1188</v>
+      </c>
+      <c r="B480" s="8" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C480" s="8" t="s">
+        <v>1190</v>
+      </c>
       <c r="D480" s="2"/>
       <c r="E480" s="2"/>
       <c r="F480" s="2"/>
@@ -17104,10 +17260,14 @@
     </row>
     <row r="481">
       <c r="A481" s="1" t="s">
-        <v>1170</v>
-      </c>
-      <c r="B481" s="2"/>
-      <c r="C481" s="2"/>
+        <v>1191</v>
+      </c>
+      <c r="B481" s="8" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C481" s="8" t="s">
+        <v>1193</v>
+      </c>
       <c r="D481" s="2"/>
       <c r="E481" s="2"/>
       <c r="F481" s="2"/>
@@ -17119,10 +17279,14 @@
     </row>
     <row r="482">
       <c r="A482" s="1" t="s">
-        <v>1171</v>
-      </c>
-      <c r="B482" s="2"/>
-      <c r="C482" s="2"/>
+        <v>1194</v>
+      </c>
+      <c r="B482" s="8" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C482" s="8" t="s">
+        <v>1195</v>
+      </c>
       <c r="D482" s="2"/>
       <c r="E482" s="2"/>
       <c r="F482" s="2"/>
@@ -17134,10 +17298,14 @@
     </row>
     <row r="483">
       <c r="A483" s="1" t="s">
-        <v>1172</v>
-      </c>
-      <c r="B483" s="2"/>
-      <c r="C483" s="2"/>
+        <v>1196</v>
+      </c>
+      <c r="B483" s="8" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C483" s="8" t="s">
+        <v>1198</v>
+      </c>
       <c r="D483" s="2"/>
       <c r="E483" s="2"/>
       <c r="F483" s="2"/>
@@ -17149,10 +17317,14 @@
     </row>
     <row r="484">
       <c r="A484" s="1" t="s">
-        <v>1173</v>
-      </c>
-      <c r="B484" s="2"/>
-      <c r="C484" s="2"/>
+        <v>1199</v>
+      </c>
+      <c r="B484" s="8" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C484" s="8" t="s">
+        <v>1201</v>
+      </c>
       <c r="D484" s="2"/>
       <c r="E484" s="2"/>
       <c r="F484" s="2"/>
@@ -17164,10 +17336,14 @@
     </row>
     <row r="485">
       <c r="A485" s="1" t="s">
-        <v>1174</v>
-      </c>
-      <c r="B485" s="2"/>
-      <c r="C485" s="2"/>
+        <v>1202</v>
+      </c>
+      <c r="B485" s="8" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C485" s="8" t="s">
+        <v>1204</v>
+      </c>
       <c r="D485" s="2"/>
       <c r="E485" s="2"/>
       <c r="F485" s="2"/>
@@ -17179,10 +17355,14 @@
     </row>
     <row r="486">
       <c r="A486" s="1" t="s">
-        <v>1175</v>
-      </c>
-      <c r="B486" s="2"/>
-      <c r="C486" s="2"/>
+        <v>1205</v>
+      </c>
+      <c r="B486" s="8" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C486" s="8" t="s">
+        <v>1207</v>
+      </c>
       <c r="D486" s="2"/>
       <c r="E486" s="2"/>
       <c r="F486" s="2"/>
@@ -17194,10 +17374,14 @@
     </row>
     <row r="487">
       <c r="A487" s="1" t="s">
-        <v>1176</v>
-      </c>
-      <c r="B487" s="2"/>
-      <c r="C487" s="2"/>
+        <v>1208</v>
+      </c>
+      <c r="B487" s="8" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C487" s="8" t="s">
+        <v>1210</v>
+      </c>
       <c r="D487" s="2"/>
       <c r="E487" s="2"/>
       <c r="F487" s="2"/>
@@ -17209,10 +17393,14 @@
     </row>
     <row r="488">
       <c r="A488" s="1" t="s">
-        <v>1177</v>
-      </c>
-      <c r="B488" s="2"/>
-      <c r="C488" s="2"/>
+        <v>1211</v>
+      </c>
+      <c r="B488" s="8" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C488" s="8" t="s">
+        <v>1213</v>
+      </c>
       <c r="D488" s="2"/>
       <c r="E488" s="2"/>
       <c r="F488" s="2"/>
@@ -17224,7 +17412,7 @@
     </row>
     <row r="489">
       <c r="A489" s="1" t="s">
-        <v>1178</v>
+        <v>1214</v>
       </c>
       <c r="B489" s="2"/>
       <c r="C489" s="2"/>
@@ -17239,7 +17427,7 @@
     </row>
     <row r="490">
       <c r="A490" s="1" t="s">
-        <v>1179</v>
+        <v>1215</v>
       </c>
       <c r="B490" s="2"/>
       <c r="C490" s="2"/>
@@ -17254,7 +17442,7 @@
     </row>
     <row r="491">
       <c r="A491" s="1" t="s">
-        <v>1180</v>
+        <v>1216</v>
       </c>
       <c r="B491" s="2"/>
       <c r="C491" s="2"/>
@@ -17269,7 +17457,7 @@
     </row>
     <row r="492">
       <c r="A492" s="1" t="s">
-        <v>1181</v>
+        <v>1217</v>
       </c>
       <c r="B492" s="2"/>
       <c r="C492" s="2"/>
@@ -17284,7 +17472,7 @@
     </row>
     <row r="493">
       <c r="A493" s="1" t="s">
-        <v>1182</v>
+        <v>1218</v>
       </c>
       <c r="B493" s="2"/>
       <c r="C493" s="2"/>
@@ -17299,7 +17487,7 @@
     </row>
     <row r="494">
       <c r="A494" s="1" t="s">
-        <v>1183</v>
+        <v>1219</v>
       </c>
       <c r="B494" s="2"/>
       <c r="C494" s="2"/>
@@ -17314,7 +17502,7 @@
     </row>
     <row r="495">
       <c r="A495" s="1" t="s">
-        <v>1184</v>
+        <v>1220</v>
       </c>
       <c r="B495" s="2"/>
       <c r="C495" s="2"/>
@@ -17329,7 +17517,7 @@
     </row>
     <row r="496">
       <c r="A496" s="1" t="s">
-        <v>1185</v>
+        <v>1221</v>
       </c>
       <c r="B496" s="2"/>
       <c r="C496" s="2"/>
@@ -17344,7 +17532,7 @@
     </row>
     <row r="497">
       <c r="A497" s="1" t="s">
-        <v>1186</v>
+        <v>1222</v>
       </c>
       <c r="B497" s="2"/>
       <c r="C497" s="2"/>
@@ -17359,7 +17547,7 @@
     </row>
     <row r="498">
       <c r="A498" s="1" t="s">
-        <v>1187</v>
+        <v>1223</v>
       </c>
       <c r="B498" s="2"/>
       <c r="C498" s="2"/>
@@ -17374,7 +17562,7 @@
     </row>
     <row r="499">
       <c r="A499" s="1" t="s">
-        <v>1188</v>
+        <v>1224</v>
       </c>
       <c r="B499" s="2"/>
       <c r="C499" s="2"/>
@@ -17389,7 +17577,7 @@
     </row>
     <row r="500">
       <c r="A500" s="1" t="s">
-        <v>1189</v>
+        <v>1225</v>
       </c>
       <c r="B500" s="2"/>
       <c r="C500" s="2"/>
@@ -17404,7 +17592,7 @@
     </row>
     <row r="501">
       <c r="A501" s="1" t="s">
-        <v>1190</v>
+        <v>1226</v>
       </c>
       <c r="B501" s="2"/>
       <c r="C501" s="2"/>
@@ -17419,7 +17607,7 @@
     </row>
     <row r="502">
       <c r="A502" s="1" t="s">
-        <v>1191</v>
+        <v>1227</v>
       </c>
       <c r="B502" s="2"/>
       <c r="C502" s="2"/>
@@ -17434,7 +17622,7 @@
     </row>
     <row r="503">
       <c r="A503" s="1" t="s">
-        <v>1192</v>
+        <v>1228</v>
       </c>
       <c r="B503" s="2"/>
       <c r="C503" s="2"/>
@@ -17449,7 +17637,7 @@
     </row>
     <row r="504">
       <c r="A504" s="1" t="s">
-        <v>1193</v>
+        <v>1229</v>
       </c>
       <c r="B504" s="2"/>
       <c r="C504" s="2"/>
@@ -17464,7 +17652,7 @@
     </row>
     <row r="505">
       <c r="A505" s="1" t="s">
-        <v>1194</v>
+        <v>1230</v>
       </c>
       <c r="B505" s="2"/>
       <c r="C505" s="2"/>
@@ -17479,7 +17667,7 @@
     </row>
     <row r="506">
       <c r="A506" s="1" t="s">
-        <v>1195</v>
+        <v>1231</v>
       </c>
       <c r="B506" s="2"/>
       <c r="C506" s="2"/>
@@ -17494,7 +17682,7 @@
     </row>
     <row r="507">
       <c r="A507" s="1" t="s">
-        <v>1196</v>
+        <v>1232</v>
       </c>
       <c r="B507" s="2"/>
       <c r="C507" s="2"/>
@@ -17509,7 +17697,7 @@
     </row>
     <row r="508">
       <c r="A508" s="1" t="s">
-        <v>1197</v>
+        <v>1233</v>
       </c>
       <c r="B508" s="2"/>
       <c r="C508" s="2"/>
@@ -17524,7 +17712,7 @@
     </row>
     <row r="509">
       <c r="A509" s="1" t="s">
-        <v>1198</v>
+        <v>1234</v>
       </c>
       <c r="B509" s="2"/>
       <c r="C509" s="2"/>
@@ -17539,7 +17727,7 @@
     </row>
     <row r="510">
       <c r="A510" s="1" t="s">
-        <v>1199</v>
+        <v>1235</v>
       </c>
       <c r="B510" s="2"/>
       <c r="C510" s="2"/>
@@ -17554,7 +17742,7 @@
     </row>
     <row r="511">
       <c r="A511" s="1" t="s">
-        <v>1200</v>
+        <v>1236</v>
       </c>
       <c r="B511" s="2"/>
       <c r="C511" s="2"/>
@@ -17569,7 +17757,7 @@
     </row>
     <row r="512">
       <c r="A512" s="1" t="s">
-        <v>1201</v>
+        <v>1237</v>
       </c>
       <c r="B512" s="2"/>
       <c r="C512" s="2"/>
@@ -17584,7 +17772,7 @@
     </row>
     <row r="513">
       <c r="A513" s="1" t="s">
-        <v>1202</v>
+        <v>1238</v>
       </c>
       <c r="B513" s="2"/>
       <c r="C513" s="2"/>
@@ -17599,7 +17787,7 @@
     </row>
     <row r="514">
       <c r="A514" s="1" t="s">
-        <v>1203</v>
+        <v>1239</v>
       </c>
       <c r="B514" s="2"/>
       <c r="C514" s="2"/>
@@ -17614,7 +17802,7 @@
     </row>
     <row r="515">
       <c r="A515" s="1" t="s">
-        <v>1204</v>
+        <v>1240</v>
       </c>
       <c r="B515" s="2"/>
       <c r="C515" s="2"/>
@@ -17629,7 +17817,7 @@
     </row>
     <row r="516">
       <c r="A516" s="1" t="s">
-        <v>1205</v>
+        <v>1241</v>
       </c>
       <c r="B516" s="2"/>
       <c r="C516" s="2"/>
@@ -17644,7 +17832,7 @@
     </row>
     <row r="517">
       <c r="A517" s="1" t="s">
-        <v>1206</v>
+        <v>1242</v>
       </c>
       <c r="B517" s="2"/>
       <c r="C517" s="2"/>
@@ -17659,7 +17847,7 @@
     </row>
     <row r="518">
       <c r="A518" s="1" t="s">
-        <v>1207</v>
+        <v>1243</v>
       </c>
       <c r="B518" s="2"/>
       <c r="C518" s="2"/>
@@ -17674,7 +17862,7 @@
     </row>
     <row r="519">
       <c r="A519" s="1" t="s">
-        <v>1208</v>
+        <v>1244</v>
       </c>
       <c r="B519" s="2"/>
       <c r="C519" s="2"/>
@@ -17689,7 +17877,7 @@
     </row>
     <row r="520">
       <c r="A520" s="1" t="s">
-        <v>1209</v>
+        <v>1245</v>
       </c>
       <c r="B520" s="2"/>
       <c r="C520" s="2"/>
@@ -17704,7 +17892,7 @@
     </row>
     <row r="521">
       <c r="A521" s="1" t="s">
-        <v>1210</v>
+        <v>1246</v>
       </c>
       <c r="B521" s="2"/>
       <c r="C521" s="2"/>
@@ -17719,7 +17907,7 @@
     </row>
     <row r="522">
       <c r="A522" s="1" t="s">
-        <v>1211</v>
+        <v>1247</v>
       </c>
       <c r="B522" s="2"/>
       <c r="C522" s="2"/>
@@ -17734,7 +17922,7 @@
     </row>
     <row r="523">
       <c r="A523" s="1" t="s">
-        <v>1212</v>
+        <v>1248</v>
       </c>
       <c r="B523" s="2"/>
       <c r="C523" s="2"/>
@@ -17749,7 +17937,7 @@
     </row>
     <row r="524">
       <c r="A524" s="1" t="s">
-        <v>1213</v>
+        <v>1249</v>
       </c>
       <c r="B524" s="2"/>
       <c r="C524" s="2"/>
@@ -17764,7 +17952,7 @@
     </row>
     <row r="525">
       <c r="A525" s="1" t="s">
-        <v>1214</v>
+        <v>1250</v>
       </c>
       <c r="B525" s="2"/>
       <c r="C525" s="2"/>
@@ -17779,7 +17967,7 @@
     </row>
     <row r="526">
       <c r="A526" s="1" t="s">
-        <v>1215</v>
+        <v>1251</v>
       </c>
       <c r="B526" s="2"/>
       <c r="C526" s="2"/>
@@ -17794,7 +17982,7 @@
     </row>
     <row r="527">
       <c r="A527" s="1" t="s">
-        <v>1216</v>
+        <v>1252</v>
       </c>
       <c r="B527" s="2"/>
       <c r="C527" s="2"/>
@@ -17809,7 +17997,7 @@
     </row>
     <row r="528">
       <c r="A528" s="1" t="s">
-        <v>1217</v>
+        <v>1253</v>
       </c>
       <c r="B528" s="2"/>
       <c r="C528" s="2"/>
@@ -17824,7 +18012,7 @@
     </row>
     <row r="529">
       <c r="A529" s="1" t="s">
-        <v>1218</v>
+        <v>1254</v>
       </c>
       <c r="B529" s="2"/>
       <c r="C529" s="2"/>
@@ -17839,7 +18027,7 @@
     </row>
     <row r="530">
       <c r="A530" s="1" t="s">
-        <v>1219</v>
+        <v>1255</v>
       </c>
       <c r="B530" s="2"/>
       <c r="C530" s="2"/>
@@ -17854,7 +18042,7 @@
     </row>
     <row r="531">
       <c r="A531" s="1" t="s">
-        <v>1220</v>
+        <v>1256</v>
       </c>
       <c r="B531" s="2"/>
       <c r="C531" s="2"/>
@@ -17869,7 +18057,7 @@
     </row>
     <row r="532">
       <c r="A532" s="1" t="s">
-        <v>1221</v>
+        <v>1257</v>
       </c>
       <c r="B532" s="2"/>
       <c r="C532" s="2"/>
@@ -17884,7 +18072,7 @@
     </row>
     <row r="533">
       <c r="A533" s="1" t="s">
-        <v>1222</v>
+        <v>1258</v>
       </c>
       <c r="B533" s="2"/>
       <c r="C533" s="2"/>
@@ -17899,7 +18087,7 @@
     </row>
     <row r="534">
       <c r="A534" s="1" t="s">
-        <v>1223</v>
+        <v>1259</v>
       </c>
       <c r="B534" s="2"/>
       <c r="C534" s="2"/>
@@ -17914,7 +18102,7 @@
     </row>
     <row r="535">
       <c r="A535" s="1" t="s">
-        <v>1224</v>
+        <v>1260</v>
       </c>
       <c r="B535" s="2"/>
       <c r="C535" s="2"/>
@@ -17929,7 +18117,7 @@
     </row>
     <row r="536">
       <c r="A536" s="1" t="s">
-        <v>1225</v>
+        <v>1261</v>
       </c>
       <c r="B536" s="2"/>
       <c r="C536" s="2"/>
@@ -17944,7 +18132,7 @@
     </row>
     <row r="537">
       <c r="A537" s="1" t="s">
-        <v>1226</v>
+        <v>1262</v>
       </c>
       <c r="B537" s="2"/>
       <c r="C537" s="2"/>
@@ -17959,7 +18147,7 @@
     </row>
     <row r="538">
       <c r="A538" s="1" t="s">
-        <v>1227</v>
+        <v>1263</v>
       </c>
       <c r="B538" s="2"/>
       <c r="C538" s="2"/>
@@ -17974,7 +18162,7 @@
     </row>
     <row r="539">
       <c r="A539" s="1" t="s">
-        <v>1228</v>
+        <v>1264</v>
       </c>
       <c r="B539" s="2"/>
       <c r="C539" s="2"/>
@@ -17989,7 +18177,7 @@
     </row>
     <row r="540">
       <c r="A540" s="1" t="s">
-        <v>1229</v>
+        <v>1265</v>
       </c>
       <c r="B540" s="2"/>
       <c r="C540" s="2"/>
@@ -18004,7 +18192,7 @@
     </row>
     <row r="541">
       <c r="A541" s="1" t="s">
-        <v>1230</v>
+        <v>1266</v>
       </c>
       <c r="B541" s="2"/>
       <c r="C541" s="2"/>
@@ -18019,7 +18207,7 @@
     </row>
     <row r="542">
       <c r="A542" s="1" t="s">
-        <v>1231</v>
+        <v>1267</v>
       </c>
       <c r="B542" s="2"/>
       <c r="C542" s="2"/>
@@ -18034,7 +18222,7 @@
     </row>
     <row r="543">
       <c r="A543" s="1" t="s">
-        <v>1232</v>
+        <v>1268</v>
       </c>
       <c r="B543" s="2"/>
       <c r="C543" s="2"/>
@@ -18049,7 +18237,7 @@
     </row>
     <row r="544">
       <c r="A544" s="1" t="s">
-        <v>1233</v>
+        <v>1269</v>
       </c>
       <c r="B544" s="2"/>
       <c r="C544" s="2"/>

</xml_diff>